<commit_message>
add targetType to SkillData.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -145,6 +145,10 @@
   </si>
   <si>
     <t>千军破</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TargetType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,56 +484,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:H23"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="9.625" customWidth="1"/>
-    <col min="7" max="7" width="10.875" customWidth="1"/>
-    <col min="8" max="8" width="11.25" customWidth="1"/>
-    <col min="12" max="12" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="9.625" customWidth="1"/>
+    <col min="8" max="8" width="10.875" customWidth="1"/>
+    <col min="9" max="9" width="11.25" customWidth="1"/>
+    <col min="13" max="13" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2">
@@ -547,15 +555,18 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3">
@@ -571,22 +582,25 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>1.2</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
@@ -599,15 +613,18 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5">
@@ -623,22 +640,25 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>1.5</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
       <c r="E6">
         <v>1</v>
       </c>
@@ -651,15 +671,18 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7">
@@ -675,22 +698,25 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
@@ -703,15 +729,18 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9">
@@ -727,43 +756,49 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>1.8</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.6</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1.2</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11">
@@ -779,17 +814,20 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12">
@@ -805,17 +843,20 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>101</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13">
@@ -831,17 +872,20 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>102</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14">
@@ -857,17 +901,20 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>103</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>1</v>
       </c>
       <c r="D15">
@@ -883,17 +930,20 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>104</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>1</v>
       </c>
       <c r="D16">
@@ -909,18 +959,21 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>105</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17">
-        <v>1</v>
+      <c r="C17" s="1">
+        <v>2</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -935,18 +988,21 @@
         <v>1</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>106</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C18">
-        <v>1</v>
+      <c r="C18" s="1">
+        <v>2</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -961,18 +1017,21 @@
         <v>1</v>
       </c>
       <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>107</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="C19" s="1">
+        <v>2</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -987,18 +1046,21 @@
         <v>1</v>
       </c>
       <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>108</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C20">
-        <v>1</v>
+      <c r="C20" s="1">
+        <v>2</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1013,18 +1075,21 @@
         <v>1</v>
       </c>
       <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>109</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C21">
-        <v>1</v>
+      <c r="C21" s="1">
+        <v>2</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1039,18 +1104,21 @@
         <v>1</v>
       </c>
       <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>110</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C22">
-        <v>1</v>
+      <c r="C22" s="1">
+        <v>2</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1065,13 +1133,16 @@
         <v>1</v>
       </c>
       <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111107" footer="0.51111111111111107"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
drawback when attacked. also some bugfix.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -222,6 +222,10 @@
   <si>
     <t>在那个时代人人都会的闪电术</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SkillType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -276,7 +280,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -285,6 +289,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -565,25 +572,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="9.625" customWidth="1"/>
-    <col min="8" max="8" width="10.875" customWidth="1"/>
-    <col min="9" max="9" width="11.25" customWidth="1"/>
-    <col min="10" max="10" width="70.875" customWidth="1"/>
-    <col min="13" max="13" width="10.5" customWidth="1"/>
-    <col min="16" max="16" width="11.625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+    <col min="5" max="7" width="9.5" customWidth="1"/>
+    <col min="8" max="8" width="9.625" customWidth="1"/>
+    <col min="9" max="9" width="10.875" customWidth="1"/>
+    <col min="10" max="10" width="11.25" customWidth="1"/>
+    <col min="11" max="11" width="70.875" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="17" max="17" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -591,31 +599,34 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -625,7 +636,7 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2">
@@ -643,11 +654,14 @@
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -655,9 +669,9 @@
         <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3">
@@ -673,13 +687,16 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -687,14 +704,14 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>1.2</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
       <c r="F4">
         <v>1</v>
       </c>
@@ -707,11 +724,14 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -719,9 +739,9 @@
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5">
@@ -737,13 +757,16 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -751,14 +774,14 @@
         <v>16</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>1.5</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
       <c r="F6">
         <v>1</v>
       </c>
@@ -771,11 +794,14 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -783,9 +809,9 @@
         <v>17</v>
       </c>
       <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7">
@@ -801,13 +827,16 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -815,14 +844,14 @@
         <v>21</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
       <c r="F8">
         <v>1</v>
       </c>
@@ -835,11 +864,14 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -847,9 +879,9 @@
         <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9">
@@ -865,13 +897,16 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -879,31 +914,34 @@
         <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10">
         <v>1.8</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.6</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1.2</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -911,9 +949,9 @@
         <v>18</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11">
@@ -929,13 +967,16 @@
         <v>1</v>
       </c>
       <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
         <v>2</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -943,9 +984,9 @@
         <v>19</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12">
@@ -961,13 +1002,16 @@
         <v>1</v>
       </c>
       <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
         <v>2</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>101</v>
       </c>
@@ -975,9 +1019,9 @@
         <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13">
@@ -993,13 +1037,16 @@
         <v>1</v>
       </c>
       <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
         <v>2</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>102</v>
       </c>
@@ -1007,9 +1054,9 @@
         <v>10</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14">
@@ -1025,13 +1072,16 @@
         <v>1</v>
       </c>
       <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
         <v>2</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>103</v>
       </c>
@@ -1039,9 +1089,9 @@
         <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15">
@@ -1057,13 +1107,16 @@
         <v>1</v>
       </c>
       <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>104</v>
       </c>
@@ -1071,9 +1124,9 @@
         <v>22</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16">
@@ -1089,13 +1142,16 @@
         <v>1</v>
       </c>
       <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
         <v>2</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>105</v>
       </c>
@@ -1103,11 +1159,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
       <c r="E17">
         <v>1</v>
       </c>
@@ -1121,13 +1177,16 @@
         <v>1</v>
       </c>
       <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
         <v>3</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>106</v>
       </c>
@@ -1135,9 +1194,9 @@
         <v>25</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18">
@@ -1153,13 +1212,16 @@
         <v>1</v>
       </c>
       <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
         <v>3</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>107</v>
       </c>
@@ -1167,11 +1229,11 @@
         <v>27</v>
       </c>
       <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
         <v>2</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
       <c r="E19">
         <v>1</v>
       </c>
@@ -1185,13 +1247,16 @@
         <v>1</v>
       </c>
       <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
         <v>3</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>108</v>
       </c>
@@ -1199,11 +1264,11 @@
         <v>26</v>
       </c>
       <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
       <c r="E20">
         <v>1</v>
       </c>
@@ -1217,13 +1282,16 @@
         <v>1</v>
       </c>
       <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
         <v>3</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>109</v>
       </c>
@@ -1231,11 +1299,11 @@
         <v>24</v>
       </c>
       <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
       <c r="E21">
         <v>1</v>
       </c>
@@ -1249,13 +1317,16 @@
         <v>1</v>
       </c>
       <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>110</v>
       </c>
@@ -1263,9 +1334,9 @@
         <v>39</v>
       </c>
       <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
         <v>1</v>
       </c>
       <c r="E22">
@@ -1281,23 +1352,26 @@
         <v>1</v>
       </c>
       <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
         <v>3</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>201</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="E23">
@@ -1313,23 +1387,26 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>202</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24">
@@ -1345,23 +1422,26 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>203</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25">
@@ -1377,9 +1457,12 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add interrupt effect. add revive effect for girl.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ChineseRoguelikeGame\Documents\ExcelData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28110" windowHeight="12630"/>
+    <workbookView windowWidth="22935" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
@@ -20,518 +15,543 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115">
+  <si>
+    <t>技能ID</t>
+  </si>
+  <si>
+    <t>技能名称</t>
+  </si>
+  <si>
+    <t>技能描述</t>
+  </si>
+  <si>
+    <t>技能类型</t>
+  </si>
+  <si>
+    <t>目标类型</t>
+  </si>
+  <si>
+    <t>攻击倍率</t>
+  </si>
+  <si>
+    <t>命中倍率</t>
+  </si>
+  <si>
+    <t>暴击倍率</t>
+  </si>
+  <si>
+    <t>前摇倍率</t>
+  </si>
+  <si>
+    <t>后摇倍率</t>
+  </si>
+  <si>
+    <t>打断倍率</t>
+  </si>
+  <si>
+    <t>最大连击</t>
+  </si>
+  <si>
+    <t>特效ID</t>
+  </si>
+  <si>
+    <t>特效出现率</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>skillType</t>
+  </si>
+  <si>
+    <t>targetType</t>
+  </si>
+  <si>
+    <t>ATKMultiplier</t>
+  </si>
+  <si>
+    <t>ACCMultiplier</t>
+  </si>
+  <si>
+    <t>CRTMultiplier</t>
+  </si>
+  <si>
+    <t>preSPDMultiplier</t>
+  </si>
+  <si>
+    <t>postSPDMultiplier</t>
+  </si>
+  <si>
+    <t>interruptMultiplier</t>
+  </si>
+  <si>
+    <t>maxCombo</t>
+  </si>
+  <si>
+    <t>buffID</t>
+  </si>
+  <si>
+    <t>buffPercentage</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>SKILLTYPE</t>
+  </si>
+  <si>
+    <t>TARGETTYPE</t>
+  </si>
+  <si>
+    <t>FLOAT</t>
+  </si>
+  <si>
     <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无招即是有招</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Melee</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>短剑轻攻击</t>
+  </si>
+  <si>
+    <t>几乎立即就可以出招的短剑轻击。</t>
+  </si>
+  <si>
+    <t>SingleEnemy</t>
+  </si>
+  <si>
+    <t>短剑重攻击</t>
+  </si>
+  <si>
+    <t>集中力量的突刺攻击。</t>
+  </si>
+  <si>
+    <t>短剑特殊技</t>
+  </si>
+  <si>
+    <t>背刺。</t>
+  </si>
+  <si>
+    <t>唐刀轻攻击</t>
+  </si>
+  <si>
+    <t>横扫。</t>
+  </si>
+  <si>
+    <t>唐刀重攻击</t>
+  </si>
+  <si>
+    <t>纵劈。</t>
+  </si>
+  <si>
+    <t>唐刀特殊技</t>
+  </si>
+  <si>
+    <t>拔刀术。</t>
+  </si>
+  <si>
+    <t>枪类轻攻击</t>
+  </si>
+  <si>
+    <t>枪类重攻击</t>
+  </si>
+  <si>
+    <t>枪类特殊技</t>
+  </si>
+  <si>
+    <t>三连击，不会暴击。</t>
+  </si>
+  <si>
+    <t>长剑轻攻击</t>
+  </si>
+  <si>
+    <t>朴实无华的轻砍。</t>
+  </si>
+  <si>
+    <t>长剑重攻击</t>
+  </si>
+  <si>
+    <t>重剑无锋的重砍。</t>
+  </si>
+  <si>
+    <t>长剑特殊技</t>
+  </si>
+  <si>
+    <t>削弱敌人的防御力。</t>
+  </si>
+  <si>
+    <t>大斧轻攻击</t>
+  </si>
+  <si>
+    <t>大斧重攻击</t>
+  </si>
+  <si>
+    <t>大斧特殊技</t>
+  </si>
+  <si>
+    <t>自身狂暴化，可能是一把双刃剑。</t>
+  </si>
+  <si>
+    <t>巨锤轻攻击</t>
+  </si>
+  <si>
+    <t>抡人。</t>
+  </si>
+  <si>
+    <t>巨锤重攻击</t>
+  </si>
+  <si>
+    <t>跳起砸地。全体攻击。</t>
+  </si>
+  <si>
+    <t>AllEnemies</t>
+  </si>
+  <si>
+    <t>巨锤特殊技</t>
+  </si>
+  <si>
+    <t>迷之旋转。全体攻击。必定击倒。</t>
+  </si>
+  <si>
+    <t>短弓轻攻击</t>
+  </si>
+  <si>
+    <t>快速射击。</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>短弓重攻击</t>
+  </si>
+  <si>
+    <t>瞄准后的一击，命中率和暴击率高。</t>
+  </si>
+  <si>
+    <t>短弓特殊技</t>
+  </si>
+  <si>
+    <t>同时射击全体，但准确度不高。</t>
+  </si>
+  <si>
+    <t>弩类轻攻击</t>
+  </si>
+  <si>
+    <t>攻击后换弹药。</t>
+  </si>
+  <si>
+    <t>弩类重攻击</t>
+  </si>
+  <si>
+    <t>将三发弹药一次击出。换弹时间长。</t>
+  </si>
+  <si>
+    <t>弩类特殊技</t>
+  </si>
+  <si>
+    <t>华丽的全体射击。</t>
+  </si>
+  <si>
+    <t>效果ID</t>
+  </si>
+  <si>
+    <t>效果名称</t>
+  </si>
+  <si>
+    <t>效果描述</t>
+  </si>
+  <si>
+    <t>持续回合</t>
+  </si>
+  <si>
+    <t>触发时机</t>
+  </si>
+  <si>
+    <t>效果函数</t>
+  </si>
+  <si>
+    <t>lastTurns</t>
+  </si>
+  <si>
+    <t>trigger</t>
+  </si>
+  <si>
+    <t>buffEffect</t>
+  </si>
+  <si>
+    <t>BUFFTRIGGER</t>
   </si>
   <si>
     <t>并没有特殊效果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>不死</t>
+  </si>
+  <si>
+    <t>无论如何也不会死亡</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Revive</t>
   </si>
   <si>
     <t>必中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无视对方回避必定命中</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lastTurns</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SingleEnemy</t>
-  </si>
-  <si>
-    <t>Self</t>
-  </si>
-  <si>
-    <t>trigger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>skillType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>targetType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Always</t>
+  </si>
+  <si>
+    <t>Hit</t>
   </si>
   <si>
     <t>MustHit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffEffect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>None</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>目标类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击倍率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>打断倍率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>命中倍率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>暴击倍率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>前摇倍率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>后摇倍率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxCombo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大连击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技能ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>特效ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短剑特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>背刺。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>几乎立即就可以出招的短剑轻击。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>buffPercentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>特效出现率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>集中力量的突刺攻击。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>唐刀特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拔刀术。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>横扫。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无法格挡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无视对方格挡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>纵劈。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>枪类重攻击</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>枪类轻攻击</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>唐刀轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>唐刀重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短剑重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短剑轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>枪类特殊技</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>长剑轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>长剑重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>长剑特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大斧轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大斧重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大斧特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>巨锤轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>巨锤重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>巨锤特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短弓轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短弓重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短弓特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弩类轻攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弩类重攻击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弩类特殊技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>枪类重攻击</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>三连击，不会暴击。</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>三连击</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>朴实无华的轻砍。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重剑无锋的重砍。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AllEnemies</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>抡人。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>跳起砸地。全体攻击。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三次伤害</t>
   </si>
   <si>
     <t>削弱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>敌减伤效果变为8</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>0%</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>削弱敌人的防御力。</t>
   </si>
   <si>
     <t>狂暴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>连续攻击同一敌人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自身狂暴化，可能是一把双刃剑。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>迷之旋转。全体攻击。必定击倒。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三次伤害</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>击倒</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>将敌人击倒，令敌人跳过下回合</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>瞄准后的一击，命中率和暴击率高。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>同时射击全体，但准确度不高。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击后换弹药。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>快速射击。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>将三发弹药一次击出。换弹时间长。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>华丽的全体射击。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>效果名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>效果描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>持续回合</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发时机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>效果函数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>效果ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STRING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STRING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STRING</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SKILLTYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TARGETTYPE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FLOAT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BUFFTRIGGER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ATKMultiplier</t>
-  </si>
-  <si>
-    <t>ACCMultiplier</t>
-  </si>
-  <si>
-    <t>CRTMultiplier</t>
-  </si>
-  <si>
-    <t>preSPDMultiplier</t>
-  </si>
-  <si>
-    <t>postSPDMultiplier</t>
-  </si>
-  <si>
-    <t>interruptMultiplier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="12"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,8 +564,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -553,9 +759,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -563,44 +1011,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -647,7 +1133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -682,7 +1168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -857,23 +1343,19 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="49.25" customWidth="1"/>
@@ -893,48 +1375,48 @@
     <col min="27" max="27" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>37</v>
+    <row r="1" spans="1:20">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -943,48 +1425,48 @@
       <c r="S1" s="4"/>
       <c r="T1" s="4"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>36</v>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
@@ -993,48 +1475,48 @@
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>100</v>
+    <row r="3" spans="1:20">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
@@ -1043,47 +1525,47 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" s="3">
+    <row r="4" spans="1:20">
+      <c r="A4" s="2">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>0</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>0</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>0</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>0</v>
       </c>
       <c r="O4" s="4"/>
@@ -1093,21 +1575,21 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20">
       <c r="A5" s="4">
         <v>1101</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
@@ -1139,21 +1621,21 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20">
       <c r="A6" s="4">
         <v>1102</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F6" s="4">
         <v>1.5</v>
@@ -1185,21 +1667,21 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20">
       <c r="A7" s="4">
         <v>1103</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F7" s="4">
         <v>6</v>
@@ -1223,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="M7" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N7" s="4">
         <v>100</v>
@@ -1235,21 +1717,21 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20">
       <c r="A8" s="4">
         <v>1201</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -1281,21 +1763,21 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20">
       <c r="A9" s="4">
         <v>1202</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F9" s="4">
         <v>1.5</v>
@@ -1327,21 +1809,21 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20">
       <c r="A10" s="4">
         <v>1203</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -1365,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="M10" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N10" s="4">
         <v>100</v>
@@ -1377,21 +1859,21 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20">
       <c r="A11" s="4">
         <v>1301</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>46</v>
+      <c r="B11" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1423,21 +1905,21 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20">
       <c r="A12" s="4">
         <v>1302</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F12" s="4">
         <v>1.5</v>
@@ -1469,21 +1951,21 @@
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20">
       <c r="A13" s="4">
         <v>1303</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>68</v>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F13" s="4">
         <v>0.7</v>
@@ -1507,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N13" s="4">
         <v>100</v>
@@ -1519,21 +2001,21 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20">
       <c r="A14" s="4">
         <v>1401</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -1565,21 +2047,21 @@
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20">
       <c r="A15" s="4">
         <v>1402</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F15" s="4">
         <v>1.5</v>
@@ -1611,21 +2093,21 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20">
       <c r="A16" s="4">
         <v>1403</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -1649,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N16" s="4">
         <v>100</v>
@@ -1661,19 +2143,19 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20">
       <c r="A17" s="4">
         <v>1501</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
@@ -1705,19 +2187,19 @@
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20">
       <c r="A18" s="4">
         <v>1502</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -1749,21 +2231,21 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20">
       <c r="A19" s="4">
         <v>1503</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
@@ -1787,7 +2269,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N19" s="4">
         <v>100</v>
@@ -1799,21 +2281,21 @@
       <c r="S19" s="4"/>
       <c r="T19" s="4"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20">
       <c r="A20" s="4">
         <v>1601</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
@@ -1845,21 +2327,21 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20">
       <c r="A21" s="4">
         <v>1602</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F21" s="4">
         <v>1.5</v>
@@ -1891,21 +2373,21 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20">
       <c r="A22" s="4">
         <v>1603</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -1929,7 +2411,7 @@
         <v>1</v>
       </c>
       <c r="M22" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N22" s="4">
         <v>100</v>
@@ -1941,21 +2423,21 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20">
       <c r="A23" s="4">
         <v>1701</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -1987,21 +2469,21 @@
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20">
       <c r="A24" s="4">
         <v>1702</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -2033,21 +2515,21 @@
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20">
       <c r="A25" s="4">
         <v>1703</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -2079,21 +2561,21 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:20">
       <c r="A26" s="4">
         <v>1801</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -2125,21 +2607,21 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20">
       <c r="A27" s="4">
         <v>1802</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F27" s="4">
         <v>0.8</v>
@@ -2163,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="M27" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N27" s="4">
         <v>100</v>
@@ -2175,21 +2657,21 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20">
       <c r="A28" s="4">
         <v>1803</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
@@ -2221,7 +2703,7 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2243,7 +2725,7 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2265,10 +2747,10 @@
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20">
       <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="4"/>
@@ -2287,10 +2769,10 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20">
       <c r="A32" s="4"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="4"/>
@@ -2309,10 +2791,10 @@
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20">
       <c r="A33" s="4"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
@@ -2332,22 +2814,22 @@
       <c r="T33" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111107" footer="0.51111111111111107"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="3" width="30.125" customWidth="1"/>
@@ -2357,225 +2839,247 @@
     <col min="7" max="8" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>43</v>
+      <c r="B6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>84</v>
+      <c r="B7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>78</v>
+      <c r="B8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>81</v>
+      <c r="B9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>86</v>
+      <c r="B10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>96</v>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51111111111111107" footer="0.51111111111111107"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor on buff system. Add SkillEffect.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
     <sheet name="Buff" sheetId="2" r:id="rId2"/>
+    <sheet name="SkillEffect" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="209">
   <si>
     <t>技能ID</t>
   </si>
@@ -130,9 +131,6 @@
     <t>Melee</t>
   </si>
   <si>
-    <t>Self</t>
-  </si>
-  <si>
     <t>SingleEnemy</t>
   </si>
   <si>
@@ -154,18 +152,12 @@
     <t>效果描述</t>
   </si>
   <si>
-    <t>持续回合</t>
-  </si>
-  <si>
     <t>触发时机</t>
   </si>
   <si>
     <t>效果函数</t>
   </si>
   <si>
-    <t>lastTurns</t>
-  </si>
-  <si>
     <t>trigger</t>
   </si>
   <si>
@@ -194,65 +186,6 @@
   </si>
   <si>
     <t>Revive</t>
-  </si>
-  <si>
-    <t>必中</t>
-  </si>
-  <si>
-    <t>无视对方回避必定命中</t>
-  </si>
-  <si>
-    <t>Hit</t>
-  </si>
-  <si>
-    <t>MustHit</t>
-  </si>
-  <si>
-    <t>无法格挡</t>
-  </si>
-  <si>
-    <t>无视对方格挡</t>
-  </si>
-  <si>
-    <t>三连击</t>
-  </si>
-  <si>
-    <t>三次伤害</t>
-  </si>
-  <si>
-    <t>削弱</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>敌减伤效果变为8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>0%</t>
-    </r>
-  </si>
-  <si>
-    <t>狂暴</t>
-  </si>
-  <si>
-    <t>连续攻击同一敌人</t>
-  </si>
-  <si>
-    <t>击倒</t>
-  </si>
-  <si>
-    <t>将敌人击倒，令敌人跳过下回合</t>
   </si>
   <si>
     <t>咩爪轻攻击</t>
@@ -712,12 +645,395 @@
     <t>“被幽灵注视着，不自觉地全身酥麻，绵软无力”</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>切换攻击</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>witchWeapon</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>witchAttack</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>瞬杀</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>背刺</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>eforeHit</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AfterDamage</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>nstantKill</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>BackStab</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>若敌人处于前摇</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>或后摇</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>时则强制命中，否则强制不中</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害强制更改为对象当前HP</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前装备武器变为空手</t>
+  </si>
+  <si>
+    <t>OnDamage</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>追加2次伤害结算</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>三连击</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>投掷</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Throw</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>吸取伤害的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>10%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>回复到自己生命</t>
+    </r>
+  </si>
+  <si>
+    <t>吸血</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>AbsorbDamage</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combo</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>effectString</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>EFFECTTRIGGER</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>兽类杀手</t>
+  </si>
+  <si>
+    <r>
+      <t>若对象带有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>兽</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>”Tag</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，则伤害</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + 25%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。若对象为灵气型，则伤害为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <t>BeastKiller</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>该回合伤害将敌方</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>置为自身</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> + 1</t>
+    </r>
+  </si>
+  <si>
+    <t>厄运一击</t>
+  </si>
+  <si>
+    <r>
+      <t>若对方</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>低于自己则有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>50%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>几率秒杀敌人，否则有</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>50%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>几率伤害自己。</t>
+    </r>
+  </si>
+  <si>
+    <t>DevilHit</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>制裁</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sanction</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>必中</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>强制命中</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MustHit</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>无视防御</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>无视对方的防御状态。命中率与伤害值照常计算</t>
+  </si>
+  <si>
+    <t>必暴击</t>
+  </si>
+  <si>
+    <t>若对方未格挡，则强制暴击</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>MustCrit</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>IgnoreDefence</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>以切换后的武器发动轻攻击一次</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -763,6 +1079,16 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -792,7 +1118,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -832,6 +1158,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1109,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -1297,7 +1638,7 @@
         <v>35</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1338,16 +1679,16 @@
         <v>1101</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
@@ -1384,16 +1725,16 @@
         <v>1102</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="4">
         <v>1.5</v>
@@ -1430,16 +1771,16 @@
         <v>1103</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="4">
         <v>6</v>
@@ -1476,16 +1817,16 @@
         <v>1104</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="4">
         <v>10</v>
@@ -1522,16 +1863,16 @@
         <v>1105</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="4">
         <v>0.5</v>
@@ -1568,16 +1909,16 @@
         <v>1106</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="4">
         <v>0.8</v>
@@ -1614,16 +1955,16 @@
         <v>1201</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1660,16 +2001,16 @@
         <v>1202</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="4">
         <v>1.2</v>
@@ -1706,16 +2047,16 @@
         <v>1203</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="4">
         <v>3</v>
@@ -1752,16 +2093,16 @@
         <v>1204</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="4">
         <v>1.2</v>
@@ -1798,16 +2139,16 @@
         <v>1205</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
@@ -1844,16 +2185,16 @@
         <v>1206</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -1890,16 +2231,16 @@
         <v>1207</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" s="4">
         <v>1.6</v>
@@ -1936,16 +2277,16 @@
         <v>1301</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -1982,16 +2323,16 @@
         <v>1302</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" s="4">
         <v>1.3</v>
@@ -2028,16 +2369,16 @@
         <v>1303</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
@@ -2074,16 +2415,16 @@
         <v>1304</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="4">
         <v>0.7</v>
@@ -2120,16 +2461,16 @@
         <v>1305</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" s="4">
         <v>1.9</v>
@@ -2166,16 +2507,16 @@
         <v>1306</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" s="4">
         <v>2.5</v>
@@ -2212,16 +2553,16 @@
         <v>1401</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -2258,16 +2599,16 @@
         <v>1402</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F25" s="4">
         <v>1.5</v>
@@ -2304,16 +2645,16 @@
         <v>1403</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F26" s="4">
         <v>1.5</v>
@@ -2350,16 +2691,16 @@
         <v>1404</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F27" s="4">
         <v>2</v>
@@ -2396,16 +2737,16 @@
         <v>1405</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F28" s="4">
         <v>0.8</v>
@@ -2442,16 +2783,16 @@
         <v>1501</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="4">
         <v>1</v>
@@ -2488,16 +2829,16 @@
         <v>1502</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F30" s="4">
         <v>1.2</v>
@@ -2534,16 +2875,16 @@
         <v>1503</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" s="4">
         <v>0.8</v>
@@ -2580,16 +2921,16 @@
         <v>1504</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F32" s="4">
         <v>1</v>
@@ -2626,16 +2967,16 @@
         <v>1505</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" s="4">
         <v>1</v>
@@ -2672,16 +3013,16 @@
         <v>1506</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F34" s="4">
         <v>0.3</v>
@@ -2718,14 +3059,14 @@
         <v>1601</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F35" s="4">
         <v>1</v>
@@ -2762,14 +3103,14 @@
         <v>1602</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F36" s="4">
         <v>1</v>
@@ -2806,16 +3147,16 @@
         <v>1603</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F37" s="4">
         <v>1</v>
@@ -2852,16 +3193,16 @@
         <v>1604</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F38" s="4">
         <v>1</v>
@@ -2898,16 +3239,16 @@
         <v>1605</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="F39" s="4">
         <v>0</v>
@@ -2944,16 +3285,16 @@
         <v>1606</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" s="4">
         <v>1</v>
@@ -2990,16 +3331,16 @@
         <v>1607</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F41" s="4">
         <v>1</v>
@@ -3036,16 +3377,16 @@
         <v>1608</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F42" s="4">
         <v>1</v>
@@ -3082,16 +3423,16 @@
         <v>1609</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" s="4">
         <v>1</v>
@@ -3128,16 +3469,16 @@
         <v>2001</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F44" s="4">
         <v>1</v>
@@ -3174,16 +3515,16 @@
         <v>2002</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
@@ -3220,16 +3561,16 @@
         <v>2003</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F46" s="4">
         <v>1</v>
@@ -3266,16 +3607,16 @@
         <v>3001</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F47" s="4">
         <v>1</v>
@@ -3312,16 +3653,16 @@
         <v>3002</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F48" s="4">
         <v>1</v>
@@ -3358,16 +3699,16 @@
         <v>3003</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F49" s="4">
         <v>1</v>
@@ -3404,16 +3745,16 @@
         <v>3004</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
@@ -3450,16 +3791,16 @@
         <v>4001</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
@@ -3496,16 +3837,16 @@
         <v>4002</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F52" s="4">
         <v>1</v>
@@ -3536,16 +3877,16 @@
         <v>4003</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F53" s="4">
         <v>1</v>
@@ -3576,16 +3917,16 @@
         <v>4004</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F54" s="4">
         <v>1</v>
@@ -3616,7 +3957,7 @@
         <v>3005</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.15">
@@ -3624,7 +3965,7 @@
         <v>3006</v>
       </c>
       <c r="B56" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.15">
@@ -3632,7 +3973,7 @@
         <v>3007</v>
       </c>
       <c r="B57" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.15">
@@ -3640,7 +3981,7 @@
         <v>4005</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.15">
@@ -3648,7 +3989,7 @@
         <v>4006</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.15">
@@ -3656,7 +3997,7 @@
         <v>3008</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.15">
@@ -3664,10 +4005,10 @@
         <v>4007</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.15">
@@ -3675,10 +4016,10 @@
         <v>3009</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.15">
@@ -3686,10 +4027,10 @@
         <v>3010</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.15">
@@ -3697,10 +4038,10 @@
         <v>3011</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
@@ -3708,10 +4049,10 @@
         <v>4008</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3724,46 +4065,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="12.75" customWidth="1"/>
     <col min="3" max="3" width="30.125" customWidth="1"/>
-    <col min="4" max="4" width="12.125" customWidth="1"/>
-    <col min="5" max="5" width="13.25" customWidth="1"/>
-    <col min="6" max="6" width="15.125" customWidth="1"/>
-    <col min="7" max="8" width="17.75" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -3774,19 +4107,13 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -3797,19 +4124,13 @@
         <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -3817,166 +4138,62 @@
         <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>60</v>
-      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3984,4 +4201,299 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="37.375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>101</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>102</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>103</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix some skill effects.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9825"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9825" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
@@ -1007,28 +1007,16 @@
     <t>烧伤</t>
   </si>
   <si>
-    <t>攻防下降50%</t>
-  </si>
-  <si>
     <t>Burnt</t>
   </si>
   <si>
     <t>中毒</t>
   </si>
   <si>
-    <t>逐渐流失生命</t>
-  </si>
-  <si>
     <t>Poison</t>
   </si>
   <si>
     <t>麻痹</t>
-  </si>
-  <si>
-    <t>命中回避暴击抗暴下降</t>
-  </si>
-  <si>
-    <t>Paralized</t>
   </si>
   <si>
     <t>击倒</t>
@@ -1603,6 +1591,22 @@
   </si>
   <si>
     <t>0</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>命中回避暴击抗暴下降</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>逐渐流失生命</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻防下降50%</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paralized</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -1731,7 +1735,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1799,6 +1803,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2078,7 +2088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
@@ -4084,7 +4094,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
@@ -4115,7 +4125,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
@@ -4146,7 +4156,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
@@ -4177,7 +4187,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
@@ -4208,7 +4218,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
@@ -4239,7 +4249,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -4270,7 +4280,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
@@ -4332,7 +4342,7 @@
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
@@ -4363,7 +4373,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
@@ -4394,7 +4404,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
@@ -4425,7 +4435,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
@@ -4443,7 +4453,7 @@
         <v>182</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>144</v>
@@ -4506,7 +4516,7 @@
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
       <c r="J59" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
@@ -4543,7 +4553,7 @@
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
@@ -4580,7 +4590,7 @@
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
@@ -4615,7 +4625,7 @@
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
       <c r="J62" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
@@ -4650,7 +4660,7 @@
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
       <c r="J63" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
@@ -4687,7 +4697,7 @@
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
       <c r="J64" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
@@ -4724,7 +4734,7 @@
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
       <c r="J65" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
@@ -4755,7 +4765,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
@@ -4786,7 +4796,7 @@
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
       <c r="J67" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
@@ -4817,7 +4827,7 @@
       <c r="H68" s="10"/>
       <c r="I68" s="10"/>
       <c r="J68" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
@@ -4848,7 +4858,7 @@
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
@@ -4866,7 +4876,7 @@
         <v>219</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>186</v>
@@ -4879,7 +4889,7 @@
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
@@ -4929,7 +4939,7 @@
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
       <c r="J72" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K72" s="10"/>
       <c r="L72" s="10"/>
@@ -4966,7 +4976,7 @@
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
       <c r="J73" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K73" s="10"/>
       <c r="L73" s="10"/>
@@ -5003,7 +5013,7 @@
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
       <c r="J74" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
@@ -5040,7 +5050,7 @@
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="19" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="K75" s="10"/>
       <c r="L75" s="10"/>
@@ -5071,7 +5081,7 @@
       <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="K76" s="10"/>
       <c r="L76" s="10"/>
@@ -5102,7 +5112,7 @@
       <c r="H77" s="10"/>
       <c r="I77" s="10"/>
       <c r="J77" s="19" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="K77" s="10"/>
       <c r="L77" s="10"/>
@@ -5133,7 +5143,7 @@
       <c r="H78" s="10"/>
       <c r="I78" s="10"/>
       <c r="J78" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
@@ -5164,7 +5174,7 @@
       <c r="H79" s="10"/>
       <c r="I79" s="10"/>
       <c r="J79" s="19" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
@@ -5195,7 +5205,7 @@
       <c r="H80" s="10"/>
       <c r="I80" s="10"/>
       <c r="J80" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
@@ -5226,7 +5236,7 @@
       <c r="H81" s="10"/>
       <c r="I81" s="10"/>
       <c r="J81" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K81" s="10"/>
       <c r="L81" s="10"/>
@@ -5257,7 +5267,7 @@
       <c r="H82" s="10"/>
       <c r="I82" s="10"/>
       <c r="J82" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
@@ -5272,7 +5282,7 @@
         <v>256</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>258</v>
@@ -5288,7 +5298,7 @@
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
       <c r="J83" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
@@ -5822,7 +5832,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -5965,7 +5975,7 @@
       <c r="D8" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="23" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5977,13 +5987,13 @@
         <v>306</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>307</v>
+        <v>403</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E9" s="22" t="s">
-        <v>308</v>
+      <c r="E9" s="24" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5991,16 +6001,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>310</v>
+        <v>402</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>311</v>
+      <c r="E10" s="24" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6008,16 +6018,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>313</v>
+        <v>401</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>314</v>
+      <c r="E11" s="24" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -6025,16 +6035,16 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C12" t="s">
-        <v>316</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>290</v>
+        <v>312</v>
+      </c>
+      <c r="D12" t="s">
+        <v>395</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -6042,16 +6052,16 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C13" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D13" t="s">
         <v>298</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6059,16 +6069,16 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C14" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D14" t="s">
         <v>298</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6076,16 +6086,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C15" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D15" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75">
@@ -6093,16 +6103,16 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C16" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D16" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6110,16 +6120,16 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C17" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D17" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6127,16 +6137,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>396</v>
+      <c r="E18" s="23" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6150,7 +6160,7 @@
         <v>101</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -6158,7 +6168,7 @@
         <v>102</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6166,7 +6176,7 @@
         <v>103</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6174,7 +6184,7 @@
         <v>104</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -6182,7 +6192,7 @@
         <v>105</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -6190,7 +6200,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6206,7 +6216,7 @@
         <v>201</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6214,7 +6224,7 @@
         <v>202</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6222,7 +6232,7 @@
         <v>203</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -6237,8 +6247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6280,7 +6290,7 @@
         <v>286</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -6294,7 +6304,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>35</v>
@@ -6311,7 +6321,7 @@
         <v>289</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>291</v>
@@ -6322,16 +6332,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -6339,16 +6349,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.5">
@@ -6359,13 +6369,13 @@
         <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -6373,16 +6383,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -6390,16 +6400,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75">
@@ -6407,16 +6417,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5">
@@ -6424,16 +6434,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
@@ -6444,13 +6454,13 @@
         <v>95</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="31.5">
@@ -6461,13 +6471,13 @@
         <v>102</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6475,16 +6485,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6498,16 +6508,16 @@
         <v>101</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6515,16 +6525,16 @@
         <v>102</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6532,16 +6542,16 @@
         <v>103</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6549,16 +6559,16 @@
         <v>104</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6566,16 +6576,16 @@
         <v>105</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.5">
@@ -6583,16 +6593,16 @@
         <v>106</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forceHit when target is self.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9825" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22935" windowHeight="9825" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
@@ -884,12 +884,6 @@
     <t>祝福</t>
   </si>
   <si>
-    <t>完全抵御下次伤害</t>
-  </si>
-  <si>
-    <t>Blessed</t>
-  </si>
-  <si>
     <t>诅咒(1)</t>
   </si>
   <si>
@@ -2057,6 +2051,14 @@
       </rPr>
       <t>00</t>
     </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blessed</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>完全抵御下次伤害</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -2747,7 +2749,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>40</v>
@@ -2784,10 +2786,10 @@
         <v>42</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>43</v>
@@ -2824,10 +2826,10 @@
         <v>44</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>43</v>
@@ -2861,13 +2863,13 @@
         <v>1103</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>373</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>374</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>375</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>43</v>
@@ -2905,19 +2907,19 @@
         <v>1104</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>378</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>380</v>
-      </c>
       <c r="D8" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -2938,10 +2940,10 @@
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
       <c r="O8" s="25" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="P8" s="25" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -2952,10 +2954,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>43</v>
@@ -2982,7 +2984,7 @@
         <v>47</v>
       </c>
       <c r="M9" s="25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N9" s="13" t="s">
         <v>49</v>
@@ -2999,13 +3001,13 @@
         <v>1106</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>43</v>
@@ -3042,10 +3044,10 @@
         <v>52</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>43</v>
@@ -3082,10 +3084,10 @@
         <v>53</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>43</v>
@@ -3122,10 +3124,10 @@
         <v>54</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>43</v>
@@ -3168,10 +3170,10 @@
         <v>57</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>58</v>
@@ -3208,10 +3210,10 @@
         <v>59</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>43</v>
@@ -3223,7 +3225,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I15" s="10">
         <v>0.7</v>
@@ -3238,10 +3240,10 @@
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -3252,10 +3254,10 @@
         <v>60</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>40</v>
@@ -3298,10 +3300,10 @@
         <v>61</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>58</v>
@@ -3342,10 +3344,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>43</v>
@@ -3382,10 +3384,10 @@
         <v>64</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>43</v>
@@ -3419,13 +3421,13 @@
         <v>1303</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>43</v>
@@ -3449,13 +3451,13 @@
         <v>1</v>
       </c>
       <c r="L20" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="N20" s="25" t="s">
         <v>348</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>349</v>
-      </c>
-      <c r="N20" s="25" t="s">
-        <v>350</v>
       </c>
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
@@ -3465,13 +3467,13 @@
         <v>1304</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>58</v>
@@ -3514,10 +3516,10 @@
         <v>66</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>43</v>
@@ -3551,13 +3553,13 @@
         <v>1306</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>43</v>
@@ -3595,13 +3597,13 @@
         <v>1401</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>43</v>
@@ -3635,13 +3637,13 @@
         <v>1402</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>43</v>
@@ -3675,13 +3677,13 @@
         <v>1403</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>43</v>
@@ -3719,13 +3721,13 @@
         <v>1404</v>
       </c>
       <c r="B27" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="D27" s="19" t="s">
         <v>411</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>413</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>72</v>
@@ -3752,10 +3754,10 @@
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
       <c r="O27" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="P27" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -3763,13 +3765,13 @@
         <v>1405</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>58</v>
@@ -3793,13 +3795,13 @@
         <v>1</v>
       </c>
       <c r="L28" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>353</v>
+      </c>
+      <c r="N28" s="19" t="s">
         <v>354</v>
-      </c>
-      <c r="M28" s="19" t="s">
-        <v>355</v>
-      </c>
-      <c r="N28" s="19" t="s">
-        <v>356</v>
       </c>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
@@ -3812,10 +3814,10 @@
         <v>74</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>43</v>
@@ -3852,10 +3854,10 @@
         <v>75</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>43</v>
@@ -3892,10 +3894,10 @@
         <v>76</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>43</v>
@@ -3933,13 +3935,13 @@
         <v>1504</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>419</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>421</v>
-      </c>
       <c r="D32" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>43</v>
@@ -3983,13 +3985,13 @@
         <v>1505</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>43</v>
@@ -4020,71 +4022,71 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>424</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="C34" s="19" t="s">
         <v>426</v>
       </c>
-      <c r="C34" s="19" t="s">
-        <v>428</v>
-      </c>
       <c r="D34" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F34" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="K34" s="19" t="s">
         <v>430</v>
       </c>
-      <c r="G34" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="J34" s="19" t="s">
-        <v>431</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>432</v>
-      </c>
       <c r="L34" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="M34" s="19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="N34" s="19" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B35" s="19" t="s">
         <v>425</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="C35" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="C35" s="19" t="s">
-        <v>429</v>
-      </c>
       <c r="D35" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H35" s="10">
         <v>1</v>
@@ -4093,19 +4095,19 @@
         <v>1</v>
       </c>
       <c r="J35" s="19" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K35" s="10">
         <v>0</v>
       </c>
       <c r="L35" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="M35" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="N35" s="19" t="s">
         <v>445</v>
-      </c>
-      <c r="M35" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="N35" s="19" t="s">
-        <v>447</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -4115,13 +4117,13 @@
         <v>1601</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>58</v>
@@ -4155,34 +4157,34 @@
         <v>1602</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>58</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K37" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
@@ -4198,28 +4200,28 @@
         <v>78</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>58</v>
       </c>
       <c r="F38" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="J38" s="19" t="s">
         <v>363</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>364</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>361</v>
-      </c>
-      <c r="I38" s="19" t="s">
-        <v>362</v>
-      </c>
-      <c r="J38" s="19" t="s">
-        <v>365</v>
       </c>
       <c r="K38" s="10">
         <v>1</v>
@@ -4235,13 +4237,13 @@
         <v>1604</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>43</v>
@@ -4275,13 +4277,13 @@
         <v>1605</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>40</v>
@@ -4318,10 +4320,10 @@
         <v>79</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>43</v>
@@ -4342,7 +4344,7 @@
         <v>0.5</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
@@ -4361,7 +4363,7 @@
         <v>81</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>43</v>
@@ -4401,7 +4403,7 @@
         <v>83</v>
       </c>
       <c r="D43" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>43</v>
@@ -4441,7 +4443,7 @@
         <v>85</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>43</v>
@@ -4509,7 +4511,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
@@ -4539,7 +4541,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
@@ -4569,7 +4571,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
@@ -4599,7 +4601,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
@@ -4629,7 +4631,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -4659,7 +4661,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
@@ -4689,7 +4691,7 @@
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -4749,7 +4751,7 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
       <c r="J54" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
@@ -4779,7 +4781,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
@@ -4809,7 +4811,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
@@ -4839,7 +4841,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
@@ -4856,7 +4858,7 @@
         <v>127</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>89</v>
@@ -4917,7 +4919,7 @@
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
       <c r="J60" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K60" s="10"/>
       <c r="L60" s="10" t="s">
@@ -4953,7 +4955,7 @@
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K61" s="10"/>
       <c r="L61" s="10" t="s">
@@ -4989,7 +4991,7 @@
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
       <c r="J62" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
@@ -5023,7 +5025,7 @@
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
       <c r="J63" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
@@ -5057,7 +5059,7 @@
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
       <c r="J64" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K64" s="10"/>
       <c r="L64" s="10" t="s">
@@ -5093,7 +5095,7 @@
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
       <c r="J65" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K65" s="10"/>
       <c r="L65" s="10" t="s">
@@ -5129,7 +5131,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
@@ -5159,7 +5161,7 @@
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
       <c r="J67" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K67" s="10"/>
       <c r="L67" s="10"/>
@@ -5189,7 +5191,7 @@
       <c r="H68" s="10"/>
       <c r="I68" s="10"/>
       <c r="J68" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
@@ -5219,7 +5221,7 @@
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
@@ -5249,7 +5251,7 @@
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
@@ -5266,7 +5268,7 @@
         <v>164</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>131</v>
@@ -5279,7 +5281,7 @@
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
       <c r="J71" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K71" s="10"/>
       <c r="L71" s="10"/>
@@ -5327,7 +5329,7 @@
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
       <c r="J73" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K73" s="10"/>
       <c r="L73" s="10" t="s">
@@ -5363,7 +5365,7 @@
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
       <c r="J74" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K74" s="10"/>
       <c r="L74" s="10" t="s">
@@ -5399,7 +5401,7 @@
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K75" s="10"/>
       <c r="L75" s="10" t="s">
@@ -5435,7 +5437,7 @@
       <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K76" s="10"/>
       <c r="L76" s="10"/>
@@ -5465,7 +5467,7 @@
       <c r="H77" s="10"/>
       <c r="I77" s="10"/>
       <c r="J77" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K77" s="10"/>
       <c r="L77" s="10"/>
@@ -5495,7 +5497,7 @@
       <c r="H78" s="10"/>
       <c r="I78" s="10"/>
       <c r="J78" s="19" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
@@ -5525,7 +5527,7 @@
       <c r="H79" s="10"/>
       <c r="I79" s="10"/>
       <c r="J79" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
@@ -5555,7 +5557,7 @@
       <c r="H80" s="10"/>
       <c r="I80" s="10"/>
       <c r="J80" s="19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
@@ -5585,7 +5587,7 @@
       <c r="H81" s="10"/>
       <c r="I81" s="10"/>
       <c r="J81" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K81" s="10"/>
       <c r="L81" s="10"/>
@@ -5615,7 +5617,7 @@
       <c r="H82" s="10"/>
       <c r="I82" s="10"/>
       <c r="J82" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
@@ -5645,7 +5647,7 @@
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
       <c r="J83" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
@@ -5659,7 +5661,7 @@
         <v>201</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>203</v>
@@ -5675,7 +5677,7 @@
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
       <c r="J84" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K84" s="10"/>
       <c r="L84" s="10"/>
@@ -5713,7 +5715,7 @@
         <v>204</v>
       </c>
       <c r="D86" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>43</v>
@@ -5753,7 +5755,7 @@
         <v>205</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>43</v>
@@ -5793,7 +5795,7 @@
         <v>206</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>43</v>
@@ -5833,7 +5835,7 @@
         <v>208</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>58</v>
@@ -5873,7 +5875,7 @@
         <v>209</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>58</v>
@@ -6179,8 +6181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6335,7 +6337,7 @@
         <v>251</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>235</v>
@@ -6352,7 +6354,7 @@
         <v>253</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>243</v>
@@ -6369,13 +6371,13 @@
         <v>255</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>235</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -6389,9 +6391,9 @@
         <v>257</v>
       </c>
       <c r="D12" t="s">
-        <v>338</v>
-      </c>
-      <c r="E12" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6437,13 +6439,13 @@
         <v>265</v>
       </c>
       <c r="C15" t="s">
-        <v>266</v>
+        <v>454</v>
       </c>
       <c r="D15" t="s">
-        <v>338</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>267</v>
+        <v>336</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75">
@@ -6451,16 +6453,16 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6468,16 +6470,16 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>268</v>
+      </c>
+      <c r="C17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" t="s">
+        <v>286</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>270</v>
-      </c>
-      <c r="C17" t="s">
-        <v>271</v>
-      </c>
-      <c r="D17" t="s">
-        <v>288</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6485,16 +6487,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>332</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>334</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>235</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6502,16 +6504,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C19" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="D19" t="s">
+        <v>336</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>351</v>
-      </c>
-      <c r="D19" t="s">
-        <v>338</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6525,7 +6527,7 @@
         <v>101</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6533,7 +6535,7 @@
         <v>102</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6541,7 +6543,7 @@
         <v>103</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -6549,7 +6551,7 @@
         <v>104</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -6557,7 +6559,7 @@
         <v>105</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6565,7 +6567,7 @@
         <v>106</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6581,7 +6583,7 @@
         <v>201</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6589,7 +6591,7 @@
         <v>202</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -6597,7 +6599,7 @@
         <v>203</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -6612,8 +6614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -6655,7 +6657,7 @@
         <v>231</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -6669,7 +6671,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>33</v>
@@ -6686,7 +6688,7 @@
         <v>234</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>236</v>
@@ -6697,16 +6699,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -6714,16 +6716,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>280</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.5">
@@ -6734,13 +6736,13 @@
         <v>45</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -6748,16 +6750,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="E8" s="21" t="s">
         <v>287</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -6765,16 +6767,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>288</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75">
@@ -6782,16 +6784,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>291</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5">
@@ -6799,16 +6801,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>294</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
@@ -6819,13 +6821,13 @@
         <v>67</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="31.5">
@@ -6836,13 +6838,13 @@
         <v>69</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6850,16 +6852,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>317</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6873,16 +6875,16 @@
         <v>101</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>301</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6890,16 +6892,16 @@
         <v>102</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6907,16 +6909,16 @@
         <v>103</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6924,16 +6926,16 @@
         <v>104</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6941,16 +6943,16 @@
         <v>105</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="28.5">
@@ -6958,16 +6960,16 @@
         <v>106</v>
       </c>
       <c r="B21" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6975,16 +6977,16 @@
         <v>107</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unify BeforeHit and OnDamage to OnHit.
</commit_message>
<xml_diff>
--- a/Documents/ExcelData/SkillData.xlsx
+++ b/Documents/ExcelData/SkillData.xlsx
@@ -893,31 +893,10 @@
     <t>EFFECTTRIGGER</t>
   </si>
   <si>
-    <t>OnDamage</t>
-  </si>
-  <si>
     <t>切换攻击</t>
   </si>
   <si>
     <t>以切换后的武器发动轻攻击一次</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>witchWeapon</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2491,6 +2470,24 @@
         <charset val="134"/>
       </rPr>
       <t>rHit</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnHit</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>witchWeapon</t>
     </r>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -3249,7 +3246,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>40</v>
@@ -3286,10 +3283,10 @@
         <v>42</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>43</v>
@@ -3326,10 +3323,10 @@
         <v>44</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>43</v>
@@ -3363,13 +3360,13 @@
         <v>1103</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>358</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>360</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>43</v>
@@ -3407,13 +3404,13 @@
         <v>1104</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C8" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>364</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>366</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>43</v>
@@ -3440,10 +3437,10 @@
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="21" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -3454,10 +3451,10 @@
         <v>46</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>43</v>
@@ -3484,7 +3481,7 @@
         <v>47</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="N9" s="12" t="s">
         <v>49</v>
@@ -3501,13 +3498,13 @@
         <v>1106</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>43</v>
@@ -3528,16 +3525,16 @@
         <v>0.2</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -3548,10 +3545,10 @@
         <v>52</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>43</v>
@@ -3588,10 +3585,10 @@
         <v>53</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>43</v>
@@ -3612,7 +3609,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
@@ -3628,10 +3625,10 @@
         <v>54</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>43</v>
@@ -3652,22 +3649,22 @@
         <v>1</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>55</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>56</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="P13" s="21" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="27">
@@ -3678,10 +3675,10 @@
         <v>57</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>58</v>
@@ -3702,7 +3699,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
@@ -3718,10 +3715,10 @@
         <v>59</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>43</v>
@@ -3742,16 +3739,16 @@
         <v>0.3</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="21" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="P15" s="21" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -3762,10 +3759,10 @@
         <v>60</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>40</v>
@@ -3808,10 +3805,10 @@
         <v>61</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>58</v>
@@ -3832,7 +3829,7 @@
         <v>0.7</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
@@ -3852,10 +3849,10 @@
         <v>63</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>43</v>
@@ -3892,10 +3889,10 @@
         <v>64</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>43</v>
@@ -3916,7 +3913,7 @@
         <v>0.5</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
@@ -3929,13 +3926,13 @@
         <v>1303</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>43</v>
@@ -3956,16 +3953,16 @@
         <v>0.3</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L20" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="N20" s="21" t="s">
         <v>334</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>336</v>
       </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
@@ -3975,13 +3972,13 @@
         <v>1304</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>58</v>
@@ -4002,7 +3999,7 @@
         <v>0.5</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L21" s="12" t="s">
         <v>65</v>
@@ -4024,10 +4021,10 @@
         <v>66</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>43</v>
@@ -4048,7 +4045,7 @@
         <v>2</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
@@ -4061,13 +4058,13 @@
         <v>1306</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>43</v>
@@ -4105,13 +4102,13 @@
         <v>1401</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E24" s="24" t="s">
         <v>43</v>
@@ -4132,7 +4129,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
@@ -4145,13 +4142,13 @@
         <v>1402</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>43</v>
@@ -4172,7 +4169,7 @@
         <v>0.7</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -4185,13 +4182,13 @@
         <v>1403</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>43</v>
@@ -4212,7 +4209,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
@@ -4229,13 +4226,13 @@
         <v>1404</v>
       </c>
       <c r="B27" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>391</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>391</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>72</v>
@@ -4256,16 +4253,16 @@
         <v>1</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -4273,13 +4270,13 @@
         <v>1405</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>58</v>
@@ -4303,13 +4300,13 @@
         <v>1</v>
       </c>
       <c r="L28" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="N28" s="17" t="s">
         <v>340</v>
-      </c>
-      <c r="M28" s="17" t="s">
-        <v>341</v>
-      </c>
-      <c r="N28" s="17" t="s">
-        <v>342</v>
       </c>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
@@ -4322,10 +4319,10 @@
         <v>74</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>43</v>
@@ -4362,10 +4359,10 @@
         <v>75</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>43</v>
@@ -4386,16 +4383,16 @@
         <v>0.8</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
       <c r="O30" s="24" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -4406,10 +4403,10 @@
         <v>76</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>43</v>
@@ -4447,13 +4444,13 @@
         <v>1504</v>
       </c>
       <c r="B32" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>399</v>
-      </c>
       <c r="D32" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>43</v>
@@ -4497,13 +4494,13 @@
         <v>1505</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>43</v>
@@ -4534,71 +4531,71 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="C34" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>406</v>
-      </c>
       <c r="D34" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F34" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>407</v>
+      </c>
+      <c r="K34" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="G34" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>410</v>
-      </c>
       <c r="L34" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="C35" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="D35" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H35" s="10">
         <v>1</v>
@@ -4607,19 +4604,19 @@
         <v>1</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K35" s="10">
         <v>0</v>
       </c>
       <c r="L35" s="17" t="s">
+        <v>421</v>
+      </c>
+      <c r="M35" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="N35" s="17" t="s">
         <v>423</v>
-      </c>
-      <c r="M35" s="17" t="s">
-        <v>424</v>
-      </c>
-      <c r="N35" s="17" t="s">
-        <v>425</v>
       </c>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -4647,13 +4644,13 @@
         <v>1601</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>58</v>
@@ -4687,34 +4684,34 @@
         <v>1602</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>58</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
@@ -4730,40 +4727,40 @@
         <v>78</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>58</v>
       </c>
       <c r="F39" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="J39" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="G39" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>351</v>
-      </c>
       <c r="K39" s="10">
         <v>1</v>
       </c>
       <c r="L39" s="17" t="s">
+        <v>464</v>
+      </c>
+      <c r="M39" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="N39" s="17" t="s">
         <v>466</v>
-      </c>
-      <c r="M39" s="17" t="s">
-        <v>467</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>468</v>
       </c>
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
@@ -4773,13 +4770,13 @@
         <v>1604</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>43</v>
@@ -4803,13 +4800,13 @@
         <v>1</v>
       </c>
       <c r="L40" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="M40" s="17" t="s">
+        <v>444</v>
+      </c>
+      <c r="N40" s="17" t="s">
         <v>445</v>
-      </c>
-      <c r="M40" s="17" t="s">
-        <v>446</v>
-      </c>
-      <c r="N40" s="17" t="s">
-        <v>447</v>
       </c>
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
@@ -4819,13 +4816,13 @@
         <v>1605</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E41" s="10" t="s">
         <v>40</v>
@@ -4849,13 +4846,13 @@
         <v>0</v>
       </c>
       <c r="L41" s="17" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
@@ -4868,10 +4865,10 @@
         <v>79</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E42" s="10" t="s">
         <v>43</v>
@@ -4892,16 +4889,16 @@
         <v>0.5</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="17" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="P42" s="17" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -4915,7 +4912,7 @@
         <v>81</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>43</v>
@@ -4942,7 +4939,7 @@
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="17" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="P43" s="10" t="s">
         <v>51</v>
@@ -4959,7 +4956,7 @@
         <v>83</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>58</v>
@@ -4986,7 +4983,7 @@
       <c r="M44" s="10"/>
       <c r="N44" s="10"/>
       <c r="O44" s="17" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="P44" s="10" t="s">
         <v>51</v>
@@ -5003,7 +5000,7 @@
         <v>85</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>99</v>
@@ -5030,7 +5027,7 @@
       <c r="M45" s="10"/>
       <c r="N45" s="10"/>
       <c r="O45" s="17" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="P45" s="10" t="s">
         <v>51</v>
@@ -5075,7 +5072,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K47" s="10"/>
       <c r="L47" s="10"/>
@@ -5105,7 +5102,7 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
@@ -5135,7 +5132,7 @@
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
@@ -5165,7 +5162,7 @@
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -5195,7 +5192,7 @@
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
@@ -5225,7 +5222,7 @@
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
       <c r="J52" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -5255,7 +5252,7 @@
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
@@ -5315,7 +5312,7 @@
       <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
@@ -5345,7 +5342,7 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
       <c r="J56" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
@@ -5375,7 +5372,7 @@
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
@@ -5405,7 +5402,7 @@
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
       <c r="J58" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
@@ -5422,7 +5419,7 @@
         <v>127</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>89</v>
@@ -5483,7 +5480,7 @@
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
       <c r="J61" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K61" s="10"/>
       <c r="L61" s="10" t="s">
@@ -5519,7 +5516,7 @@
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
       <c r="J62" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="10" t="s">
@@ -5555,7 +5552,7 @@
       <c r="H63" s="10"/>
       <c r="I63" s="10"/>
       <c r="J63" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
@@ -5589,7 +5586,7 @@
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
       <c r="J64" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
@@ -5623,7 +5620,7 @@
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
       <c r="J65" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K65" s="10"/>
       <c r="L65" s="10" t="s">
@@ -5659,7 +5656,7 @@
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
       <c r="J66" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K66" s="10"/>
       <c r="L66" s="10" t="s">
@@ -5695,17 +5692,17 @@
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
       <c r="J67" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K67" s="10"/>
       <c r="L67" s="17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M67" s="17" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N67" s="17" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
@@ -5731,7 +5728,7 @@
       <c r="H68" s="10"/>
       <c r="I68" s="10"/>
       <c r="J68" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
@@ -5761,7 +5758,7 @@
       <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
@@ -5791,7 +5788,7 @@
       <c r="H70" s="10"/>
       <c r="I70" s="10"/>
       <c r="J70" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
@@ -5821,7 +5818,7 @@
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
       <c r="J71" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K71" s="10"/>
       <c r="L71" s="10"/>
@@ -5838,7 +5835,7 @@
         <v>164</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D72" s="10" t="s">
         <v>131</v>
@@ -5851,7 +5848,7 @@
       <c r="H72" s="10"/>
       <c r="I72" s="10"/>
       <c r="J72" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K72" s="10"/>
       <c r="L72" s="10"/>
@@ -5899,7 +5896,7 @@
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
       <c r="J74" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K74" s="10"/>
       <c r="L74" s="10" t="s">
@@ -5935,7 +5932,7 @@
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K75" s="10"/>
       <c r="L75" s="10" t="s">
@@ -5971,7 +5968,7 @@
       <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K76" s="10"/>
       <c r="L76" s="10" t="s">
@@ -6007,7 +6004,7 @@
       <c r="H77" s="10"/>
       <c r="I77" s="10"/>
       <c r="J77" s="17" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K77" s="10"/>
       <c r="L77" s="10"/>
@@ -6037,7 +6034,7 @@
       <c r="H78" s="10"/>
       <c r="I78" s="10"/>
       <c r="J78" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K78" s="10"/>
       <c r="L78" s="17"/>
@@ -6067,17 +6064,17 @@
       <c r="H79" s="10"/>
       <c r="I79" s="10"/>
       <c r="J79" s="17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K79" s="10"/>
       <c r="L79" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="M79" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="N79" s="17" t="s">
         <v>471</v>
-      </c>
-      <c r="M79" s="17" t="s">
-        <v>472</v>
-      </c>
-      <c r="N79" s="17" t="s">
-        <v>473</v>
       </c>
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
@@ -6103,7 +6100,7 @@
       <c r="H80" s="10"/>
       <c r="I80" s="10"/>
       <c r="J80" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K80" s="10"/>
       <c r="L80" s="17"/>
@@ -6133,7 +6130,7 @@
       <c r="H81" s="10"/>
       <c r="I81" s="10"/>
       <c r="J81" s="17" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K81" s="10"/>
       <c r="L81" s="10"/>
@@ -6163,7 +6160,7 @@
       <c r="H82" s="10"/>
       <c r="I82" s="10"/>
       <c r="J82" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
@@ -6193,7 +6190,7 @@
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
       <c r="J83" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
@@ -6223,17 +6220,17 @@
       <c r="H84" s="10"/>
       <c r="I84" s="10"/>
       <c r="J84" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K84" s="10"/>
       <c r="L84" s="17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="M84" s="17" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="N84" s="17" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
@@ -6243,7 +6240,7 @@
         <v>201</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>203</v>
@@ -6259,7 +6256,7 @@
       <c r="H85" s="10"/>
       <c r="I85" s="10"/>
       <c r="J85" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K85" s="10"/>
       <c r="L85" s="10"/>
@@ -6297,7 +6294,7 @@
         <v>204</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>43</v>
@@ -6337,7 +6334,7 @@
         <v>205</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>43</v>
@@ -6377,7 +6374,7 @@
         <v>206</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>43</v>
@@ -6417,7 +6414,7 @@
         <v>208</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>58</v>
@@ -6457,7 +6454,7 @@
         <v>209</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>58</v>
@@ -6919,7 +6916,7 @@
         <v>251</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>235</v>
@@ -6936,7 +6933,7 @@
         <v>253</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>243</v>
@@ -6953,13 +6950,13 @@
         <v>255</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>235</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -6973,7 +6970,7 @@
         <v>257</v>
       </c>
       <c r="D12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>258</v>
@@ -7021,13 +7018,13 @@
         <v>265</v>
       </c>
       <c r="C15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D15" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7035,16 +7032,16 @@
         <v>12</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="D16" t="s">
+        <v>322</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>337</v>
-      </c>
-      <c r="D16" t="s">
-        <v>324</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7052,16 +7049,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C17" t="s">
         <v>266</v>
       </c>
       <c r="D17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7069,16 +7066,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>235</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -7092,7 +7089,7 @@
         <v>101</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7100,7 +7097,7 @@
         <v>102</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -7108,7 +7105,7 @@
         <v>103</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -7116,7 +7113,7 @@
         <v>104</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7124,7 +7121,7 @@
         <v>105</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -7132,7 +7129,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -7148,7 +7145,7 @@
         <v>201</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -7156,7 +7153,7 @@
         <v>202</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -7164,7 +7161,7 @@
         <v>203</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -7180,7 +7177,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -7253,7 +7250,7 @@
         <v>234</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>269</v>
+        <v>492</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>236</v>
@@ -7264,16 +7261,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7281,16 +7278,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.5">
@@ -7301,13 +7298,13 @@
         <v>45</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7315,16 +7312,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="E8" s="30" t="s">
         <v>280</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>493</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75">
@@ -7332,16 +7329,16 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>491</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>283</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>493</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="31.5">
@@ -7349,16 +7346,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>286</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75">
@@ -7369,13 +7366,13 @@
         <v>67</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="31.5">
@@ -7386,13 +7383,13 @@
         <v>69</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -7400,16 +7397,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>454</v>
-      </c>
       <c r="D13" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -7417,16 +7414,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="16" t="s">
+        <v>453</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>454</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>455</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>456</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -7434,16 +7431,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7457,16 +7454,16 @@
         <v>101</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -7474,16 +7471,16 @@
         <v>102</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -7491,16 +7488,16 @@
         <v>103</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -7508,16 +7505,16 @@
         <v>104</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>300</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -7525,16 +7522,16 @@
         <v>105</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>303</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.5">
@@ -7542,16 +7539,16 @@
         <v>106</v>
       </c>
       <c r="B22" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -7559,16 +7556,16 @@
         <v>107</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -7576,16 +7573,16 @@
         <v>108</v>
       </c>
       <c r="B24" s="16" t="s">
+        <v>475</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>476</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>477</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>478</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>492</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>